<commit_message>
EPBDS-7627 Incorrect Cast happens if ternary operator is used
--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7627_ifnodebinder_with_customspreadsheetresult.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7627_ifnodebinder_with_customspreadsheetresult.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr documentId="13_ncr:1_{6A3E2AF7-8B7E-4ECF-92E5-C5478599B3BF}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
+    <workbookView windowHeight="13350" windowWidth="27795" xWindow="480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="EPBDS-7777" sheetId="1" r:id="rId1"/>
+    <sheet name="EPBDS-7777" r:id="rId1" sheetId="1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <r>
       <t xml:space="preserve">Spreadsheet SpreadsheetResult </t>
@@ -155,11 +161,54 @@
   <si>
     <t>= value</t>
   </si>
+  <si>
+    <t>Val1</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Res1</t>
+  </si>
+  <si>
+    <t>= $TTT.$Formula$Val1</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult DetermineHouseGrossSocietyPremium ( DoubleValue value)</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult DetermineContentsGrossSocietyPremium ( DoubleValue value )</t>
+  </si>
+  <si>
+    <t>= instanceOf($TTT.$Formula$Val1, Object.class)</t>
+  </si>
+  <si>
+    <t>_res_.$Formula$Res1</t>
+  </si>
+  <si>
+    <t>Expected1</t>
+  </si>
+  <si>
+    <t>Res2</t>
+  </si>
+  <si>
+    <t>= instanceOf($TTT.$Formula$Val1, DoubleValue.class)</t>
+  </si>
+  <si>
+    <t>_res_.$Formula$Res2</t>
+  </si>
+  <si>
+    <t>Expected2</t>
+  </si>
+  <si>
+    <t>= instanceOf($TTT.$Formula$Val, DoubleValue.class)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -177,13 +226,13 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="000000" theme="1"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="0" tint="-0.34998626667073579"/>
+      <color rgb="FFFFFF" theme="0" tint="-0.34998626667073579"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
     </font>
@@ -195,7 +244,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="000000" theme="1"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <charset val="204"/>
@@ -217,7 +266,7 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="000000" theme="1"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
     </font>
@@ -262,37 +311,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor rgb="FFFFFF" theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor rgb="4F81BD" theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFFF" theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14996795556505021"/>
+        <fgColor rgb="FFFFFF" theme="0" tint="-0.14996795556505021"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FFFFFF" theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59996337778862885"/>
+        <fgColor rgb="4F81BD" theme="4" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,111 +422,98 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0">
-      <alignment horizontal="left"/>
-    </xf>
+  <cellStyleXfs count="7">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="3"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="4"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="5"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="6"/>
   </cellStyleXfs>
   <cellXfs count="22">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="2">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="3">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="5" numFmtId="0" quotePrefix="1" xfId="4"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="4"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="6" fontId="7" numFmtId="0" xfId="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="8" fontId="7" numFmtId="0" quotePrefix="1" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="6" fontId="3" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="6" fontId="3" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="5"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="5">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="6">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="6"/>
+    <xf applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="6"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="9" fontId="4" numFmtId="0" xfId="6">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="0" fillId="10" fontId="4" numFmtId="0" xfId="2">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="6" fontId="8" numFmtId="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="8" fontId="8" numFmtId="0" quotePrefix="1" xfId="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="14">
-    <cellStyle name=" 1" xfId="4"/>
-    <cellStyle name="20% - Accent1 2 13" xfId="7"/>
-    <cellStyle name="20% - Accent1 2 16" xfId="3"/>
-    <cellStyle name="20% - Accent1 2 4 2 3" xfId="8"/>
-    <cellStyle name="20% - Accent1 2 4 3 3" xfId="9"/>
-    <cellStyle name="20% - Accent1 2 6" xfId="2"/>
-    <cellStyle name="20% - Accent1 3" xfId="6"/>
-    <cellStyle name="20% - Accent2 2" xfId="10"/>
-    <cellStyle name="20% - Accent6 2 4 3 2" xfId="11"/>
-    <cellStyle name="Comma 19 2 5" xfId="1"/>
-    <cellStyle name="Datatype" xfId="12"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10 14" xfId="13"/>
-    <cellStyle name="Normal 2" xfId="5"/>
+  <cellStyles count="7">
+    <cellStyle builtinId="0" name="Обычный" xfId="0"/>
+    <cellStyle name="Comma 19 2 5" xfId="1" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="20% - Accent1 2 6" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="20% - Accent1 2 16" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name=" 1" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="20% - Accent1 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -510,9 +546,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -545,9 +581,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -580,9 +633,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -635,7 +705,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -644,13 +714,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -660,7 +730,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -669,7 +739,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -678,7 +748,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -688,12 +758,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -724,7 +794,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -743,7 +813,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -755,93 +825,109 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:K35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.140625" style="1" collapsed="1"/>
-    <col min="3" max="3" width="36.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="93.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="52" style="3" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="47.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="35" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="33.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="37.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="9.140625" style="1"/>
-    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="2" max="2" style="1" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="36.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="93.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="52.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="47.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="35.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="33.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="37.42578125" collapsed="true"/>
+    <col min="10" max="11" style="1" width="9.140625" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="21"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="C5" s="6" t="s">
+    <row customFormat="1" ht="15" r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="C6" s="9" t="s">
+      <c r="A6" s="7"/>
+      <c r="C6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C14" s="11" t="s">
+    <row r="7">
+      <c r="C7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row ht="15" r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
       <c r="F14"/>
       <c r="G14"/>
       <c r="H14"/>
       <c r="I14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="14">
         <v>1</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-    </row>
-    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C16" s="17" t="s">
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+    </row>
+    <row ht="15" r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="14">
         <v>1.1000000000000001</v>
       </c>
       <c r="F16"/>
@@ -849,94 +935,116 @@
       <c r="H16"/>
       <c r="I16"/>
     </row>
-    <row r="17" spans="3:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
+    <row ht="15" r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="14" t="b">
+        <v>1</v>
+      </c>
       <c r="F17"/>
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17"/>
     </row>
+    <row r="18">
+      <c r="C18" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="C23" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="1"/>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="3:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="3:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="D25" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row ht="15" r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row ht="15" r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
     </row>
-    <row r="28" spans="3:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="C29" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="1"/>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="21" t="s">
+      <c r="D31" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="3:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="3:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row ht="15" r="32" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="20" t="str">
+        <f> "Hello"</f>
+        <v>Hello</v>
+      </c>
+    </row>
+    <row ht="15" r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="3:5" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C34"/>
       <c r="D34"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="3:5" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="35" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C35"/>
       <c r="D35"/>
       <c r="E35"/>
@@ -944,10 +1052,10 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C29:D29"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-7627 Incorrect Cast happens if ternary operator is used - Add new test
--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7627_ifnodebinder_with_customspreadsheetresult.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7627_ifnodebinder_with_customspreadsheetresult.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{6A3E2AF7-8B7E-4ECF-92E5-C5478599B3BF}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37"/>
   <bookViews>
-    <workbookView windowHeight="13350" windowWidth="27795" xWindow="480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="30"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="27795" windowHeight="13290" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="EPBDS-7777" r:id="rId1" sheetId="1"/>
+    <sheet name="EPBDS-7777" sheetId="1" r:id="rId1"/>
+    <sheet name="Test2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
   <si>
     <r>
       <t xml:space="preserve">Spreadsheet SpreadsheetResult </t>
@@ -110,70 +105,18 @@
     <t>Expected</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Spreadsheet SpreadsheetResult </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-      </rPr>
-      <t>DetermineHouseGrossSocietyPremium</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ( DoubleValue value)</t>
-    </r>
-  </si>
-  <si>
     <t>Val</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Spreadsheet SpreadsheetResult </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-      </rPr>
-      <t>DetermineContentsGrossSocietyPremium</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ( DoubleValue value )</t>
-    </r>
-  </si>
-  <si>
     <t>= value</t>
   </si>
   <si>
     <t>Val1</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Res1</t>
   </si>
   <si>
-    <t>= $TTT.$Formula$Val1</t>
-  </si>
-  <si>
     <t>Spreadsheet SpreadsheetResult DetermineHouseGrossSocietyPremium ( DoubleValue value)</t>
   </si>
   <si>
@@ -192,9 +135,6 @@
     <t>Res2</t>
   </si>
   <si>
-    <t>= instanceOf($TTT.$Formula$Val1, DoubleValue.class)</t>
-  </si>
-  <si>
     <t>_res_.$Formula$Res2</t>
   </si>
   <si>
@@ -202,14 +142,136 @@
   </si>
   <si>
     <t>= instanceOf($TTT.$Formula$Val, DoubleValue.class)</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult a()</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>DoubleVal</t>
+  </si>
+  <si>
+    <t>= 10.0</t>
+  </si>
+  <si>
+    <t>CastVal</t>
+  </si>
+  <si>
+    <t>=10</t>
+  </si>
+  <si>
+    <t>StringVal</t>
+  </si>
+  <si>
+    <t>="123"</t>
+  </si>
+  <si>
+    <t>SomeVal1</t>
+  </si>
+  <si>
+    <t>= 12.0</t>
+  </si>
+  <si>
+    <t>=3.3</t>
+  </si>
+  <si>
+    <t>=123</t>
+  </si>
+  <si>
+    <t>="10"</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult b()</t>
+  </si>
+  <si>
+    <t>=(x &gt;0 )? a().$Values$DoubleVal : b().$Values$DoubleVal</t>
+  </si>
+  <si>
+    <t>spType</t>
+  </si>
+  <si>
+    <t>DoubleValCheck</t>
+  </si>
+  <si>
+    <t>=(x &gt;0 )? a().$Values$CastVal : b().$Values$CastVal</t>
+  </si>
+  <si>
+    <t>CastValCheck</t>
+  </si>
+  <si>
+    <t>=(x &gt;0 )? a().$Values$StringVal : b().$Values$StringVal</t>
+  </si>
+  <si>
+    <t>StringValCheck</t>
+  </si>
+  <si>
+    <t>=instanceOf($Values$DoubleValCheck, Double.class)</t>
+  </si>
+  <si>
+    <t>=instanceOf($Values$CastValCheck, Double.class)</t>
+  </si>
+  <si>
+    <t>=instanceOf($Values$StringValCheck, Double.class)</t>
+  </si>
+  <si>
+    <t>StringValCheck2</t>
+  </si>
+  <si>
+    <t>=instanceOf($Values$StringValCheck, Object.class)</t>
+  </si>
+  <si>
+    <t>SomeValCheck</t>
+  </si>
+  <si>
+    <t>=(x &gt;0 )? a().$Values$SomeVal1 : b().$Values$SomeVal1</t>
+  </si>
+  <si>
+    <t>=instanceOf($Values$StringValCheck, String.class)</t>
+  </si>
+  <si>
+    <t>=instanceOf($Values$StringValCheck, Integer.class)</t>
+  </si>
+  <si>
+    <t>SomeValCheck2</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult checkTrenarycast(Integer x)</t>
+  </si>
+  <si>
+    <t>Test checkTrenarycast</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>_res_.$spType$DoubleValCheck</t>
+  </si>
+  <si>
+    <t>_res_.$spType$CastValCheck</t>
+  </si>
+  <si>
+    <t>_res_.$spType$StringValCheck</t>
+  </si>
+  <si>
+    <t>_res_.$spType$StringValCheck2</t>
+  </si>
+  <si>
+    <t>_res_.$spType$SomeValCheck</t>
+  </si>
+  <si>
+    <t>_res_.$spType$SomeValCheck2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,13 +288,13 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="000000" theme="1"/>
+      <color theme="1"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFFFF" theme="0" tint="-0.34998626667073579"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
     </font>
@@ -244,7 +306,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="000000" theme="1"/>
+      <color theme="1"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <charset val="204"/>
@@ -266,42 +328,17 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color rgb="000000" theme="1"/>
-      <name val="Franklin Gothic Book"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="186"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <color theme="1"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -311,37 +348,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF" theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="4F81BD" theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF" theme="0"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF" theme="0" tint="-0.14996795556505021"/>
+        <fgColor theme="0" tint="-0.14996795556505021"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF" theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="4F81BD" theme="4" tint="0.59996337778862885"/>
+        <fgColor theme="4" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,77 +460,112 @@
     </border>
   </borders>
   <cellStyleXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="3"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="4"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="5"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
+  <cellXfs count="25">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="2">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="3">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="5" numFmtId="0" quotePrefix="1" xfId="4"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="4"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="6" fontId="7" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="8" fontId="7" numFmtId="0" quotePrefix="1" xfId="1"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="6" fontId="3" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="6" fontId="3" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="5"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="5">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="6">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="6"/>
-    <xf applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="6"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="9" fontId="4" numFmtId="0" xfId="6">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="0" fillId="10" fontId="4" numFmtId="0" xfId="2">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="6" fontId="8" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="8" fontId="8" numFmtId="0" quotePrefix="1" xfId="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle builtinId="0" name="Обычный" xfId="0"/>
-    <cellStyle name="Comma 19 2 5" xfId="1" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="20% - Accent1 2 6" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="20% - Accent1 2 16" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name=" 1" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="20% - Accent1 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name=" 1" xfId="4"/>
+    <cellStyle name="20% - Accent1 2 16" xfId="3"/>
+    <cellStyle name="20% - Accent1 2 6" xfId="2"/>
+    <cellStyle name="20% - Accent1 3" xfId="6"/>
+    <cellStyle name="Comma 19 2 5" xfId="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -506,14 +578,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -546,9 +618,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -581,26 +653,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -633,26 +688,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -705,7 +743,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -714,13 +752,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -730,7 +768,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -739,7 +777,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -748,7 +786,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -758,12 +796,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -794,7 +832,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -813,7 +851,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -825,33 +863,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:J35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="2" max="2" style="1" width="9.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="36.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="93.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="52.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="47.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="35.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="33.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="37.42578125" collapsed="true"/>
-    <col min="10" max="11" style="1" width="9.140625" collapsed="true"/>
-    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.140625" style="1" collapsed="1"/>
+    <col min="3" max="3" width="36.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="93.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="52" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="47.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="35" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="33.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="37.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="21"/>
+      <c r="D3" s="22"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
@@ -861,7 +898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customFormat="1" ht="15" r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
@@ -878,23 +915,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row ht="15" r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="C14" s="10" t="s">
         <v>7</v>
       </c>
@@ -920,7 +957,7 @@
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
     </row>
-    <row ht="15" r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="C16" s="16" t="s">
         <v>10</v>
       </c>
@@ -935,12 +972,12 @@
       <c r="H16"/>
       <c r="I16"/>
     </row>
-    <row ht="15" r="17" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:9" ht="15" x14ac:dyDescent="0.25">
       <c r="C17" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E17" s="14" t="b">
         <v>1</v>
@@ -950,22 +987,22 @@
       <c r="H17"/>
       <c r="I17"/>
     </row>
-    <row r="18">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" s="16" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E18" s="14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="21"/>
+      <c r="C23" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="22"/>
       <c r="E23" s="21"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
@@ -978,35 +1015,35 @@
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C25" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row ht="15" r="26" spans="3:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26" s="19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row ht="15" r="27" spans="3:9" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" ht="15" x14ac:dyDescent="0.25">
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
     </row>
-    <row ht="15" r="28" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:9" ht="15" x14ac:dyDescent="0.25">
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C29" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="21"/>
+      <c r="C29" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="22"/>
       <c r="E29" s="21"/>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
@@ -1019,32 +1056,32 @@
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C31" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row ht="15" r="32" spans="3:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C32" s="19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D32" s="20" t="str">
-        <f> "Hello"</f>
+        <f>"Hello"</f>
         <v>Hello</v>
       </c>
     </row>
-    <row ht="15" r="33" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:5" ht="15" x14ac:dyDescent="0.25">
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33" s="1"/>
     </row>
-    <row ht="15" r="34" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:5" ht="15" x14ac:dyDescent="0.25">
       <c r="C34"/>
       <c r="D34"/>
       <c r="E34" s="1"/>
     </row>
-    <row ht="15" r="35" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:5" ht="15" x14ac:dyDescent="0.25">
       <c r="C35"/>
       <c r="D35"/>
       <c r="E35"/>
@@ -1055,7 +1092,301 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C29:D29"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:H34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="53.140625" customWidth="1"/>
+    <col min="4" max="5" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="30" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" customWidth="1"/>
+    <col min="8" max="8" width="30.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="23"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="23"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="23"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" t="s">
+        <v>64</v>
+      </c>
+      <c r="H31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" t="s">
+        <v>64</v>
+      </c>
+      <c r="H32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" t="b">
+        <v>0</v>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B20:C20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>